<commit_message>
Added Wiki and updated UI with RA and LP plots working
</commit_message>
<xml_diff>
--- a/model_data.xlsx
+++ b/model_data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="994" firstSheet="0" activeTab="33"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="994" firstSheet="0" activeTab="34"/>
   </bookViews>
   <sheets>
     <sheet name="SYS1" sheetId="1" state="visible" r:id="rId2"/>
@@ -42,13 +42,14 @@
     <sheet name="DATA13" sheetId="32" state="visible" r:id="rId33"/>
     <sheet name="DATA14" sheetId="33" state="visible" r:id="rId34"/>
     <sheet name="JM_Results" sheetId="34" state="visible" r:id="rId35"/>
+    <sheet name="GM_Results" sheetId="35" state="visible" r:id="rId36"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="51">
   <si>
     <t>FN</t>
   </si>
@@ -131,10 +132,10 @@
     <t>J4</t>
   </si>
   <si>
-    <t>1.5471490664958912*^16 </t>
+    <t>1.5471490664958912*^16</t>
   </si>
   <si>
-    <t>1.0682534013936593*^-16 </t>
+    <t>1.0682534013936593*^-16</t>
   </si>
   <si>
     <t>J5</t>
@@ -158,10 +159,10 @@
     <t>DATA3</t>
   </si>
   <si>
-    <t>2.5999787083264925*^15 </t>
+    <t>2.5999787083264925*^15</t>
   </si>
   <si>
-    <t>8.630464672030806*^-16 </t>
+    <t>8.630464672030806*^-16</t>
   </si>
   <si>
     <t>DATA4</t>
@@ -182,10 +183,10 @@
     <t>DATA9</t>
   </si>
   <si>
-    <t>4.820292029641751*^15 </t>
+    <t>4.820292029641751*^15</t>
   </si>
   <si>
-    <t>6.252107987658547*^-17 </t>
+    <t>6.252107987658547*^-17</t>
   </si>
   <si>
     <t>DATA10</t>
@@ -310,7 +311,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="3" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="6" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -23955,8 +23956,8 @@
   </sheetPr>
   <dimension ref="A1:B181"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A52" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B69" activeCellId="0" sqref="B69"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A38" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D120" activeCellId="0" sqref="D120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -24508,7 +24509,7 @@
         <v>42.589</v>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="n">
         <v>68</v>
       </c>
@@ -27759,14 +27760,14 @@
   </sheetPr>
   <dimension ref="A1:C32"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.2857142857143"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.2857142857143"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="34.7091836734694"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.9948979591837"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.4183673469388"/>
   </cols>
@@ -28101,7 +28102,7 @@
         <v>0.00466305300880831</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="6" t="s">
         <v>49</v>
       </c>
@@ -28112,12 +28113,12 @@
         <v>0.00446722718489859</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="6" t="s">
         <v>50</v>
       </c>
       <c r="B32" s="0" t="n">
-        <v>343.622159930298</v>
+        <v>379.451893534383</v>
       </c>
       <c r="C32" s="0" t="n">
         <v>0.0274737343527539</v>
@@ -28126,6 +28127,379 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C65536"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.72959183673469"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="11.9948979591837"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.72959183673469"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="0" t="n">
+        <v>0.977114771748347</v>
+      </c>
+      <c r="C1" s="0" t="n">
+        <v>0.0106303732494466</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>0.980482093366516</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>0.00217717010034645</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>0.992412571914574</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>0.0303113057923857</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>0.996287349900077</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>15.5500415001421</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>0.996120779904461</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>0.00914265109969296</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>0.997468462346952</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>0.00508595691281129</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>0.933136299630931</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>0.00323315599695973</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>0.942079045780052</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>0.00352966783955137</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>0.997196222376023</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>2.60886540452676</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>0.997398728851271</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>1.70198008709158</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <v>0.996325606679967</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>18.1597071079486</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" s="0" t="n">
+        <v>1.00499530016353</v>
+      </c>
+      <c r="C12" s="0" t="n">
+        <v>1.08583720007116</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" s="0" t="n">
+        <v>0.999296653995539</v>
+      </c>
+      <c r="C13" s="0" t="n">
+        <v>5.74813763360032</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" s="0" t="n">
+        <v>0.966571646780011</v>
+      </c>
+      <c r="C14" s="0" t="n">
+        <v>0.0548838225841933</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" s="0" t="n">
+        <v>0.977248844781959</v>
+      </c>
+      <c r="C15" s="0" t="n">
+        <v>0.0108873886542901</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="B16" s="0" t="n">
+        <v>1.00778468081251</v>
+      </c>
+      <c r="C16" s="0" t="n">
+        <v>1.89619632021729</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="B17" s="0" t="n">
+        <v>0.996985444572247</v>
+      </c>
+      <c r="C17" s="0" t="n">
+        <v>11.9714348723793</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="B18" s="0" t="n">
+        <v>0.994138096439638</v>
+      </c>
+      <c r="C18" s="0" t="n">
+        <v>55.674127860977</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="B19" s="0" t="n">
+        <v>0.999716097908601</v>
+      </c>
+      <c r="C19" s="0" t="n">
+        <v>404.806439000878</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="B20" s="0" t="n">
+        <v>0.997329645200844</v>
+      </c>
+      <c r="C20" s="0" t="n">
+        <v>11.457400725189</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="B21" s="0" t="n">
+        <v>0.995941406393821</v>
+      </c>
+      <c r="C21" s="0" t="n">
+        <v>14.8038340894198</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="B22" s="0" t="n">
+        <v>1.00737706092221</v>
+      </c>
+      <c r="C22" s="0" t="n">
+        <v>0.249422030325261</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="B23" s="0" t="n">
+        <v>0.999440070997736</v>
+      </c>
+      <c r="C23" s="0" t="n">
+        <v>13.2939404152746</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="B24" s="0" t="n">
+        <v>0.988334003271029</v>
+      </c>
+      <c r="C24" s="0" t="n">
+        <v>3.10461190626825</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="B25" s="0" t="n">
+        <v>0.99530194855462</v>
+      </c>
+      <c r="C25" s="0" t="n">
+        <v>1.73955024969013</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="B26" s="0" t="n">
+        <v>0.994289298581167</v>
+      </c>
+      <c r="C26" s="0" t="n">
+        <v>1.90029801143342</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B27" s="0" t="n">
+        <v>0.995857731358413</v>
+      </c>
+      <c r="C27" s="0" t="n">
+        <v>11.1060742290678</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B28" s="0" t="n">
+        <v>0.990864746776967</v>
+      </c>
+      <c r="C28" s="0" t="n">
+        <v>0.0416559068111573</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B29" s="0" t="n">
+        <v>0.976393361670496</v>
+      </c>
+      <c r="C29" s="0" t="n">
+        <v>0.0102250435748306</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B30" s="0" t="n">
+        <v>0.974832650587054</v>
+      </c>
+      <c r="C30" s="0" t="n">
+        <v>0.0318841814426526</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B31" s="0" t="n">
+        <v>0.996325606679967</v>
+      </c>
+      <c r="C31" s="0" t="n">
+        <v>18.1597071079486</v>
+      </c>
+    </row>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>

</xml_diff>

<commit_message>
MVF plot works of FC data too now[implicit conversion based on input data
</commit_message>
<xml_diff>
--- a/model_data.xlsx
+++ b/model_data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="994" firstSheet="0" activeTab="34"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="994" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="SYS1" sheetId="1" state="visible" r:id="rId2"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="50">
   <si>
     <t>FN</t>
   </si>
@@ -63,7 +63,7 @@
     <t>FT (ms)</t>
   </si>
   <si>
-    <t>TI</t>
+    <t>T</t>
   </si>
   <si>
     <t>FC</t>
@@ -76,9 +76,6 @@
   </si>
   <si>
     <t>FT(n 1000)</t>
-  </si>
-  <si>
-    <t>T</t>
   </si>
   <si>
     <t>IT</t>
@@ -311,7 +308,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="6" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="3" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -2028,7 +2025,7 @@
   <dimension ref="A1:C42"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -2558,7 +2555,7 @@
   <dimension ref="A1:C115"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -3964,7 +3961,7 @@
   <dimension ref="A1:C74"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -6250,7 +6247,7 @@
   <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -7249,7 +7246,7 @@
   <dimension ref="A1:C82"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -11371,7 +11368,7 @@
   <dimension ref="A1:C42"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -11387,7 +11384,7 @@
         <v>5</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11900,7 +11897,7 @@
   </sheetPr>
   <dimension ref="A1:C87"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
@@ -12981,7 +12978,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B1" s="0" t="s">
         <v>6</v>
@@ -13271,7 +13268,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B1" s="0" t="s">
         <v>6</v>
@@ -13635,7 +13632,7 @@
   <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H21" activeCellId="0" sqref="H21"/>
+      <selection pane="topLeft" activeCell="C21" activeCellId="0" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -13645,7 +13642,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B1" s="0" t="s">
         <v>6</v>
@@ -13654,7 +13651,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
         <v>1</v>
       </c>
@@ -13666,7 +13663,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
         <v>2</v>
       </c>
@@ -13678,7 +13675,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
         <v>3</v>
       </c>
@@ -13690,7 +13687,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
         <v>4</v>
       </c>
@@ -13702,7 +13699,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
         <v>6</v>
       </c>
@@ -13714,7 +13711,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
         <v>7</v>
       </c>
@@ -13726,7 +13723,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
         <v>8</v>
       </c>
@@ -13738,7 +13735,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
         <v>9</v>
       </c>
@@ -13750,7 +13747,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
         <v>10</v>
       </c>
@@ -13762,7 +13759,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
         <v>11</v>
       </c>
@@ -13774,7 +13771,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
         <v>12</v>
       </c>
@@ -13786,7 +13783,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
         <v>13</v>
       </c>
@@ -13798,7 +13795,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="n">
         <v>14</v>
       </c>
@@ -13810,7 +13807,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="n">
         <v>15</v>
       </c>
@@ -13822,7 +13819,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="n">
         <v>16</v>
       </c>
@@ -13834,7 +13831,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="n">
         <v>17</v>
       </c>
@@ -13846,7 +13843,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="n">
         <v>18</v>
       </c>
@@ -13858,7 +13855,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="n">
         <v>19</v>
       </c>
@@ -13870,7 +13867,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="n">
         <v>20</v>
       </c>
@@ -13882,7 +13879,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="n">
         <v>21</v>
       </c>
@@ -13929,10 +13926,10 @@
         <v>6</v>
       </c>
       <c r="C1" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="0" t="s">
         <v>9</v>
-      </c>
-      <c r="D1" s="0" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14274,7 +14271,7 @@
         <v>6</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14432,7 +14429,7 @@
         <v>6</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14620,7 +14617,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B1" s="0" t="s">
         <v>6</v>
@@ -15966,7 +15963,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B1" s="0" t="s">
         <v>6</v>
@@ -17335,7 +17332,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B1" s="0" t="s">
         <v>6</v>
@@ -19767,7 +19764,7 @@
         <v>6</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -22519,7 +22516,7 @@
         <v>6</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23956,7 +23953,7 @@
   </sheetPr>
   <dimension ref="A1:B181"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A38" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D120" activeCellId="0" sqref="D120"/>
     </sheetView>
   </sheetViews>
@@ -23970,7 +23967,7 @@
         <v>6</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -25445,7 +25442,7 @@
         <v>6</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -27170,7 +27167,7 @@
   </sheetPr>
   <dimension ref="A1:C47"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A18" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E26" activeCellId="0" sqref="E26"/>
     </sheetView>
   </sheetViews>
@@ -27187,7 +27184,7 @@
         <v>6</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -27774,18 +27771,18 @@
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C1" s="4" t="s">
         <v>12</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>141.902891867447</v>
@@ -27796,7 +27793,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>105.012807228783</v>
@@ -27807,7 +27804,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>254.133340764334</v>
@@ -27818,7 +27815,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>525.594576714226</v>
@@ -27829,7 +27826,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>397.482742089856</v>
@@ -27840,7 +27837,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>458.313357092745</v>
@@ -27851,7 +27848,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>400.406070734606</v>
@@ -27862,7 +27859,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>132.295309709242</v>
@@ -27873,7 +27870,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>116.614534193463</v>
@@ -27884,7 +27881,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>394.982363232817</v>
@@ -27895,7 +27892,7 @@
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>341.395996917092</v>
@@ -27906,7 +27903,7 @@
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>416.017507983375</v>
@@ -27917,18 +27914,18 @@
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="B14" s="0" t="s">
+      <c r="C14" s="0" t="s">
         <v>27</v>
-      </c>
-      <c r="C14" s="0" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>1539.00334573189</v>
@@ -27939,7 +27936,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B16" s="0" t="n">
         <v>56.0991410917235</v>
@@ -27950,7 +27947,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B17" s="0" t="n">
         <v>42.1960066511982</v>
@@ -27961,7 +27958,7 @@
     </row>
     <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>416.017507983375</v>
@@ -27972,7 +27969,7 @@
     </row>
     <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B19" s="0" t="n">
         <v>52.1575464989474</v>
@@ -27983,7 +27980,7 @@
     </row>
     <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B20" s="0" t="n">
         <v>141.891901738625</v>
@@ -27994,18 +27991,18 @@
     </row>
     <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B21" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="B21" s="0" t="s">
+      <c r="C21" s="0" t="s">
         <v>36</v>
-      </c>
-      <c r="C21" s="0" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B22" s="0" t="n">
         <v>465.546093269026</v>
@@ -28016,7 +28013,7 @@
     </row>
     <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B23" s="0" t="n">
         <v>324.504920638012</v>
@@ -28027,7 +28024,7 @@
     </row>
     <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B24" s="0" t="n">
         <v>4957.80270036686</v>
@@ -28038,7 +28035,7 @@
     </row>
     <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B25" s="0" t="n">
         <v>603.959409845491</v>
@@ -28049,7 +28046,7 @@
     </row>
     <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B26" s="0" t="n">
         <v>496.898362453637</v>
@@ -28060,18 +28057,18 @@
     </row>
     <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B27" s="0" t="s">
         <v>43</v>
       </c>
-      <c r="B27" s="0" t="s">
+      <c r="C27" s="0" t="s">
         <v>44</v>
-      </c>
-      <c r="C27" s="0" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B28" s="0" t="n">
         <v>1382.87894465423</v>
@@ -28082,7 +28079,7 @@
     </row>
     <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B29" s="0" t="n">
         <v>158.935027089395</v>
@@ -28093,7 +28090,7 @@
     </row>
     <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B30" s="0" t="n">
         <v>339.049863128139</v>
@@ -28104,7 +28101,7 @@
     </row>
     <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B31" s="0" t="n">
         <v>343.622159930298</v>
@@ -28115,7 +28112,7 @@
     </row>
     <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B32" s="0" t="n">
         <v>379.451893534383</v>
@@ -28142,7 +28139,7 @@
   </sheetPr>
   <dimension ref="A1:C65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
     </sheetView>
   </sheetViews>
@@ -28155,7 +28152,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B1" s="0" t="n">
         <v>0.977114771748347</v>
@@ -28166,7 +28163,7 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>0.980482093366516</v>
@@ -28177,7 +28174,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>0.992412571914574</v>
@@ -28188,7 +28185,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>0.996287349900077</v>
@@ -28199,7 +28196,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>0.996120779904461</v>
@@ -28210,7 +28207,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>0.997468462346952</v>
@@ -28221,7 +28218,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>0.933136299630931</v>
@@ -28232,7 +28229,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>0.942079045780052</v>
@@ -28243,7 +28240,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>0.997196222376023</v>
@@ -28254,7 +28251,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>0.997398728851271</v>
@@ -28265,7 +28262,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>0.996325606679967</v>
@@ -28276,7 +28273,7 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>1.00499530016353</v>
@@ -28287,7 +28284,7 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>0.999296653995539</v>
@@ -28298,7 +28295,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>0.966571646780011</v>
@@ -28309,7 +28306,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>0.977248844781959</v>
@@ -28320,7 +28317,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B16" s="0" t="n">
         <v>1.00778468081251</v>
@@ -28331,7 +28328,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B17" s="0" t="n">
         <v>0.996985444572247</v>
@@ -28342,7 +28339,7 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>0.994138096439638</v>
@@ -28353,7 +28350,7 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B19" s="0" t="n">
         <v>0.999716097908601</v>
@@ -28364,7 +28361,7 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B20" s="0" t="n">
         <v>0.997329645200844</v>
@@ -28375,7 +28372,7 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B21" s="0" t="n">
         <v>0.995941406393821</v>
@@ -28386,7 +28383,7 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B22" s="0" t="n">
         <v>1.00737706092221</v>
@@ -28397,7 +28394,7 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B23" s="0" t="n">
         <v>0.999440070997736</v>
@@ -28408,7 +28405,7 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B24" s="0" t="n">
         <v>0.988334003271029</v>
@@ -28419,7 +28416,7 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B25" s="0" t="n">
         <v>0.99530194855462</v>
@@ -28430,7 +28427,7 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B26" s="0" t="n">
         <v>0.994289298581167</v>
@@ -28441,7 +28438,7 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B27" s="0" t="n">
         <v>0.995857731358413</v>
@@ -28452,7 +28449,7 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B28" s="0" t="n">
         <v>0.990864746776967</v>
@@ -28463,7 +28460,7 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B29" s="0" t="n">
         <v>0.976393361670496</v>
@@ -28474,7 +28471,7 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B30" s="0" t="n">
         <v>0.974832650587054</v>
@@ -28485,7 +28482,7 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B31" s="0" t="n">
         <v>0.996325606679967</v>
@@ -40679,7 +40676,7 @@
   <dimension ref="A1:C63"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -41461,7 +41458,7 @@
   <dimension ref="A1:C182"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>

</xml_diff>